<commit_message>
Technically version 0.4. Sending it to JLCPCB for production.
</commit_message>
<xml_diff>
--- a/PCB/mainPCB/mainPCB-BOM-v0_4-00.xlsx
+++ b/PCB/mainPCB/mainPCB-BOM-v0_4-00.xlsx
@@ -12,12 +12,12 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$28</definedName>
-    <definedName name="bomExported" localSheetId="0">Sheet1!$B$1:$Z$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$Z$28</definedName>
+    <definedName name="bomExported" localSheetId="0">BOM!$B$1:$Z$28</definedName>
     <definedName name="mainPCB" localSheetId="1">Sheet2!$A$1:$F$42</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -206,9 +206,6 @@
     <t>R5, R8, R11, R17, R25, R40, R43, R46, R49</t>
   </si>
   <si>
-    <t>10uF</t>
-  </si>
-  <si>
     <t>1.0UF50V10%(1206)</t>
   </si>
   <si>
@@ -762,6 +759,9 @@
   </si>
   <si>
     <t>import mainPCB.mnt in dirctory</t>
+  </si>
+  <si>
+    <t>1uF</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1115,7 @@
   <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1165,13 +1165,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>5</v>
@@ -1237,10 +1237,10 @@
         <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="I2" s="2">
         <v>0.22</v>
@@ -1276,10 +1276,10 @@
         <v>28</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I3" s="2">
         <v>0.1</v>
@@ -1317,10 +1317,10 @@
         <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="I4" s="2">
         <v>0.1</v>
@@ -1358,10 +1358,10 @@
         <v>35</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I5" s="2">
         <v>0.5</v>
@@ -1399,10 +1399,10 @@
         <v>39</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I6" s="2">
         <v>0.1</v>
@@ -1446,10 +1446,10 @@
         <v>42</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="I7" s="2">
         <v>0.1</v>
@@ -1475,26 +1475,26 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1506,10 +1506,10 @@
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="V8" t="s">
+        <v>46</v>
+      </c>
+      <c r="W8" t="s">
         <v>47</v>
-      </c>
-      <c r="W8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
@@ -1520,26 +1520,26 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1559,7 +1559,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>30</v>
@@ -1568,13 +1568,13 @@
         <v>31</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
@@ -1607,13 +1607,13 @@
         <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
@@ -1637,28 +1637,28 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I12" s="2">
         <v>0.91</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -1687,13 +1687,13 @@
         <v>31</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="I13" s="2">
         <v>0.1</v>
@@ -1719,7 +1719,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>30</v>
@@ -1728,13 +1728,13 @@
         <v>31</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="I14" s="2">
         <v>0.1</v>
@@ -1760,28 +1760,28 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I15" s="2">
         <v>2.42</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1801,49 +1801,49 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I16" s="2">
         <v>0.69</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S16" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
@@ -1854,28 +1854,28 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I17" s="2">
         <v>0.22</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1887,7 +1887,7 @@
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="V17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
@@ -1898,28 +1898,28 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="G18" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="I18" s="2">
         <v>0.22</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1939,22 +1939,22 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1964,13 +1964,13 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="X19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
@@ -1981,60 +1981,60 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="G20" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I20" s="2">
         <v>0.46</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="S20" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S20" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>34</v>
@@ -2043,7 +2043,7 @@
         <v>1206</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2069,22 +2069,22 @@
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I22" s="2">
         <v>0.68</v>
@@ -2096,39 +2096,39 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="X22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -2142,33 +2142,33 @@
     </row>
     <row r="24" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -2177,7 +2177,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="Y24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -2188,50 +2188,50 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I25" s="2">
         <v>3.65</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S25" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="R25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S25" s="2" t="s">
+      <c r="U25" t="s">
         <v>119</v>
-      </c>
-      <c r="U25" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
@@ -2242,28 +2242,28 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="G26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="I26" s="2">
         <v>3.32</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -2283,50 +2283,50 @@
         <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I27" s="2">
         <v>1.17</v>
       </c>
       <c r="J27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="S27" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="R27" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="S27" s="2" t="s">
+      <c r="U27" t="s">
         <v>130</v>
-      </c>
-      <c r="U27" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -2337,28 +2337,28 @@
         <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="G28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="I28" s="2">
         <v>1.03</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -2403,50 +2403,50 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1">
         <v>20.02</v>
@@ -2464,7 +2464,7 @@
         <v>36</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K3" s="1">
         <v>1</v>
@@ -2472,7 +2472,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="1">
         <v>76.84</v>
@@ -2490,7 +2490,7 @@
         <v>36</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="1">
         <v>79.12</v>
@@ -2516,7 +2516,7 @@
         <v>36</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1">
         <v>81.28</v>
@@ -2542,7 +2542,7 @@
         <v>36</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K6" s="1">
         <v>1</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="1">
         <v>82.17</v>
@@ -2568,7 +2568,7 @@
         <v>36</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="1">
         <v>90.3</v>
@@ -2594,7 +2594,7 @@
         <v>36</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K8" s="1">
         <v>1</v>
@@ -2602,7 +2602,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" s="1">
         <v>91.31</v>
@@ -2620,7 +2620,7 @@
         <v>36</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K9" s="1">
         <v>1</v>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="1">
         <v>93.34</v>
@@ -2646,7 +2646,7 @@
         <v>36</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K10" s="1">
         <v>1</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="1">
         <v>95.89</v>
@@ -2672,18 +2672,18 @@
         <v>36</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K11" s="1">
         <v>1</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12" s="1">
         <v>76.53</v>
@@ -2701,7 +2701,7 @@
         <v>36</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K12" s="1">
         <v>1</v>
@@ -2709,7 +2709,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13" s="1">
         <v>76.53</v>
@@ -2727,7 +2727,7 @@
         <v>36</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K13" s="1">
         <v>1</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" s="1">
         <v>22.02</v>
@@ -2750,10 +2750,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K14" s="1">
         <v>1</v>
@@ -2761,7 +2761,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15" s="1">
         <v>44.5</v>
@@ -2776,10 +2776,10 @@
         <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K15" s="1">
         <v>1</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="1">
         <v>67.87</v>
@@ -2802,10 +2802,10 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K16" s="1">
         <v>1</v>
@@ -2813,7 +2813,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="1">
         <v>89.71</v>
@@ -2828,10 +2828,10 @@
         <v>1</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K17" s="1">
         <v>1</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="1">
         <v>113.33</v>
@@ -2854,10 +2854,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K18" s="1">
         <v>1</v>
@@ -2865,7 +2865,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B19" s="1">
         <v>135.94</v>
@@ -2880,10 +2880,10 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K19" s="1">
         <v>1</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B20" s="1">
         <v>159.05000000000001</v>
@@ -2906,10 +2906,10 @@
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K20" s="1">
         <v>1</v>
@@ -2917,7 +2917,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B21" s="1">
         <v>180.42</v>
@@ -2932,10 +2932,10 @@
         <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K21" s="1">
         <v>1</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B22" s="1">
         <v>36.96</v>
@@ -2961,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K22" s="1">
         <v>1</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B23" s="1">
         <v>39.880000000000003</v>
@@ -2987,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K23" s="1">
         <v>1</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24" s="1">
         <v>64.260000000000005</v>
@@ -3013,7 +3013,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K24" s="1">
         <v>1</v>
@@ -3021,7 +3021,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B25" s="1">
         <v>34.04</v>
@@ -3039,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K25" s="1">
         <v>1</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B26" s="1">
         <v>57.96</v>
@@ -3073,7 +3073,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B27" s="1">
         <v>76.53</v>
@@ -3091,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K27" s="1">
         <v>1</v>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B28" s="1">
         <v>93.42</v>
@@ -3117,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K28" s="1">
         <v>1</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" s="1">
         <v>10.11</v>
@@ -3140,10 +3140,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K29" s="1">
         <v>1</v>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B30" s="1">
         <v>10.11</v>
@@ -3166,10 +3166,10 @@
         <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K30" s="1">
         <v>1</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B31" s="1">
         <v>10.11</v>
@@ -3192,10 +3192,10 @@
         <v>1</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K31" s="1">
         <v>1</v>
@@ -3203,7 +3203,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B32" s="1">
         <v>184.15</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B33" s="1">
         <v>79.63</v>
@@ -3247,7 +3247,7 @@
         <v>330</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K33" s="1">
         <v>1</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B34" s="1">
         <v>82.04</v>
@@ -3273,7 +3273,7 @@
         <v>330</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K34" s="1">
         <v>1</v>
@@ -3281,7 +3281,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B35" s="1">
         <v>84.07</v>
@@ -3299,7 +3299,7 @@
         <v>330</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K35" s="1">
         <v>1</v>
@@ -3307,7 +3307,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B36" s="1">
         <v>84.84</v>
@@ -3325,7 +3325,7 @@
         <v>330</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K36" s="1">
         <v>1</v>
@@ -3333,7 +3333,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B37" s="1">
         <v>87.63</v>
@@ -3351,7 +3351,7 @@
         <v>330</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K37" s="1">
         <v>1</v>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B38" s="1">
         <v>88.52</v>
@@ -3377,7 +3377,7 @@
         <v>330</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K38" s="1">
         <v>1</v>
@@ -3385,7 +3385,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B39" s="1">
         <v>90.55</v>
@@ -3403,7 +3403,7 @@
         <v>330</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K39" s="1">
         <v>1</v>
@@ -3411,7 +3411,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B40" s="1">
         <v>93.22</v>
@@ -3429,7 +3429,7 @@
         <v>330</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K40" s="1">
         <v>1</v>
@@ -3437,7 +3437,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" s="1">
         <v>86.23</v>
@@ -3452,10 +3452,10 @@
         <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K41" s="1">
         <v>1</v>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42" s="1">
         <v>20.02</v>
@@ -3478,10 +3478,10 @@
         <v>1</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K42" s="1">
         <v>1</v>

</xml_diff>